<commit_message>
doing my best to get this hydrophone stuff done!!
</commit_message>
<xml_diff>
--- a/Hydrophones/recordings_summary.xlsx
+++ b/Hydrophones/recordings_summary.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Hydrophones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Hydrophones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6996B3-B8AF-401B-8580-EFC164C0ABBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B58FF1B-6B28-41AA-AB2E-2109439BB2F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{175391B8-8C03-49AB-B2ED-5D2F1A1D2F6B}"/>
+    <workbookView xWindow="-25320" yWindow="360" windowWidth="25440" windowHeight="15270" xr2:uid="{175391B8-8C03-49AB-B2ED-5D2F1A1D2F6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Impact Pipe" sheetId="1" r:id="rId1"/>
-    <sheet name="Hydrophone" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="43">
   <si>
     <t>Flood1</t>
   </si>
@@ -72,12 +72,6 @@
     <t xml:space="preserve">Tracer Data? </t>
   </si>
   <si>
-    <t>Baseflow Q</t>
-  </si>
-  <si>
-    <t>Peak Q</t>
-  </si>
-  <si>
     <t>Sediment Impact?</t>
   </si>
   <si>
@@ -154,6 +148,24 @@
   </si>
   <si>
     <t>High flow events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes* </t>
+  </si>
+  <si>
+    <t>Impact Time</t>
+  </si>
+  <si>
+    <t>Yes*</t>
+  </si>
+  <si>
+    <t>Baseflow tau</t>
+  </si>
+  <si>
+    <t>Peak tau</t>
+  </si>
+  <si>
+    <t>Time Peak tau</t>
   </si>
 </sst>
 </file>
@@ -161,9 +173,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="167" formatCode="h:mm:ss;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +211,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,21 +249,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="19" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -256,9 +270,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,121 +614,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEE0009-6E2E-409C-BC5C-11CC45C1060F}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" customWidth="1"/>
-    <col min="7" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2">
         <v>23</v>
@@ -728,16 +749,16 @@
         <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I4" s="1">
         <v>30</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -748,16 +769,16 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="1"/>
@@ -766,16 +787,16 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="1"/>
@@ -783,336 +804,539 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="10">
+        <v>242</v>
+      </c>
+      <c r="C10" s="1">
+        <v>200</v>
+      </c>
+      <c r="D10" s="1">
+        <v>318</v>
+      </c>
+      <c r="E10" s="1">
+        <v>706</v>
+      </c>
+      <c r="F10" s="1">
+        <v>112</v>
+      </c>
+      <c r="G10" s="1">
+        <v>265</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="1">
+        <v>217</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="9">
+        <v>45189</v>
+      </c>
+      <c r="C11" s="4">
+        <v>45189</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45189</v>
+      </c>
+      <c r="E11" s="4">
+        <v>45190</v>
+      </c>
+      <c r="F11" s="4">
+        <v>45190</v>
+      </c>
+      <c r="G11" s="4">
+        <v>45191</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="4">
+        <v>45191</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="11">
+        <v>0.54053240740740738</v>
+      </c>
+      <c r="C12" s="12">
+        <v>0.58097222222222222</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.63141203703703708</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.44289351851851849</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.47629629629629627</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.50723379629629628</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.62417824074074069</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="14">
-        <v>242</v>
-      </c>
-      <c r="C9" s="1">
-        <v>200</v>
-      </c>
-      <c r="D9" s="1">
-        <v>318</v>
-      </c>
-      <c r="E9" s="1">
-        <v>706</v>
-      </c>
-      <c r="F9" s="8">
-        <v>112</v>
-      </c>
-      <c r="G9" s="1">
-        <v>265</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="1">
-        <v>217</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="13">
-        <v>45189</v>
-      </c>
-      <c r="C10" s="5">
-        <v>45189</v>
-      </c>
-      <c r="D10" s="3">
-        <v>45189</v>
-      </c>
-      <c r="E10" s="5">
-        <v>45190</v>
-      </c>
-      <c r="F10" s="5">
-        <v>45190</v>
-      </c>
-      <c r="G10" s="5">
-        <v>45191</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="5">
-        <v>45191</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="15">
-        <v>0.54053240740740738</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.58097222222222222</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0.63141203703703708</v>
-      </c>
-      <c r="E11" s="7">
-        <v>0.44289351851851849</v>
-      </c>
-      <c r="F11" s="7">
-        <v>0.47629629629629627</v>
-      </c>
-      <c r="G11" s="7">
-        <v>0.50723379629629628</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="7">
-        <v>0.62417824074074069</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+      <c r="B18" s="2">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1">
+        <v>30</v>
+      </c>
+      <c r="E18" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="12" t="s">
+      <c r="F18" s="1">
+        <v>23</v>
+      </c>
+      <c r="G18" s="1">
+        <v>23</v>
+      </c>
+      <c r="H18" s="1">
+        <v>23</v>
+      </c>
+      <c r="I18" s="1">
         <v>30</v>
       </c>
-      <c r="D14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="J18" s="1">
+        <v>30</v>
+      </c>
+      <c r="K18" s="1">
+        <v>30</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2">
-        <v>30</v>
-      </c>
-      <c r="C17" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>17</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="B22" s="2"/>
       <c r="C22" s="1"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D22" s="1"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="13">
+        <v>11</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="9">
         <v>44400</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C24" s="4">
         <v>44776</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D24" s="4">
         <v>44781</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E24" s="9">
         <v>45136</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F24" s="4">
         <v>45151</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G24" s="4">
         <v>45166</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H24" s="4">
         <v>45183</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I24" s="4">
         <v>45046</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J24" s="4">
         <v>45047</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K24" s="4">
         <v>45049</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L24" s="4">
         <v>45050</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="5">
+        <v>0.61527777777777781</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="5">
+        <v>0.51094907407407408</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="5">
+        <v>0.73995370370370372</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.68798611111111108</v>
+      </c>
+      <c r="K25" s="5">
+        <v>0.6877199074074074</v>
+      </c>
+      <c r="L25" s="5">
+        <v>0.96875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0.61527777777777781</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="1"/>
+      <c r="E26" s="14"/>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E27" s="14"/>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B98C1C33-059D-4B65-AAEA-B5F68BA74840}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AB6F01-B377-4CA3-A96C-452FADD6C5A1}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>